<commit_message>
Primeiro commit — sincronizando com GitHub
</commit_message>
<xml_diff>
--- a/backend/Relatorios/EQUIPAMENTOS.xlsx
+++ b/backend/Relatorios/EQUIPAMENTOS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a7c850682481644d/Área de Trabalho/Dados/Manutenção/Dashboard Manutenção/PCM Hub/backend/Cubos/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a7c850682481644d/Área de Trabalho/Dados/Manutenção/Dashboard Manutenção/PCM-Hub/backend/Relatorios/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="99" documentId="8_{ACEEC684-1EFE-4448-A728-C2B86633E31A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{294BC36F-DDDF-4C44-86D1-5F468C177E79}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{C6CAF68A-D8F8-4870-81F4-4FC02A730870}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8DED1412-F60F-4BE0-BB0F-30E15E59F6E7}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{9A298B7C-2CFB-4F34-BA94-2821FA60F8C6}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="24240" windowHeight="13020" xr2:uid="{9A298B7C-2CFB-4F34-BA94-2821FA60F8C6}"/>
   </bookViews>
   <sheets>
     <sheet name="equipamentos" sheetId="1" r:id="rId1"/>
@@ -9220,12 +9220,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -9241,10 +9240,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -9566,7 +9561,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17250C8F-BCBF-4003-A46A-DD871B9C78D0}">
   <dimension ref="A1:K2325"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
@@ -9642,7 +9637,7 @@
       <c r="I2">
         <v>10</v>
       </c>
-      <c r="J2" s="2">
+      <c r="J2">
         <v>2021</v>
       </c>
       <c r="K2" t="s">
@@ -9677,7 +9672,7 @@
       <c r="I3">
         <v>10</v>
       </c>
-      <c r="J3" s="2">
+      <c r="J3">
         <v>2021</v>
       </c>
       <c r="K3" t="s">
@@ -9712,7 +9707,7 @@
       <c r="I4">
         <v>10</v>
       </c>
-      <c r="J4" s="2">
+      <c r="J4">
         <v>2021</v>
       </c>
       <c r="K4" t="s">
@@ -9747,7 +9742,7 @@
       <c r="I5">
         <v>10</v>
       </c>
-      <c r="J5" s="2">
+      <c r="J5">
         <v>2021</v>
       </c>
       <c r="K5" t="s">
@@ -9782,7 +9777,7 @@
       <c r="I6">
         <v>10</v>
       </c>
-      <c r="J6" s="2">
+      <c r="J6">
         <v>2021</v>
       </c>
       <c r="K6" t="s">
@@ -9817,7 +9812,7 @@
       <c r="I7">
         <v>10</v>
       </c>
-      <c r="J7" s="2">
+      <c r="J7">
         <v>2021</v>
       </c>
       <c r="K7" t="s">
@@ -9852,7 +9847,7 @@
       <c r="I8">
         <v>10</v>
       </c>
-      <c r="J8" s="2">
+      <c r="J8">
         <v>2024</v>
       </c>
       <c r="K8" t="s">
@@ -9887,7 +9882,7 @@
       <c r="I9">
         <v>10</v>
       </c>
-      <c r="J9" s="2">
+      <c r="J9">
         <v>2024</v>
       </c>
       <c r="K9" t="s">
@@ -9922,7 +9917,7 @@
       <c r="I10">
         <v>10</v>
       </c>
-      <c r="J10" s="2">
+      <c r="J10">
         <v>2024</v>
       </c>
       <c r="K10" t="s">
@@ -9957,7 +9952,7 @@
       <c r="I11">
         <v>10</v>
       </c>
-      <c r="J11" s="2">
+      <c r="J11">
         <v>2024</v>
       </c>
       <c r="K11" t="s">
@@ -9992,7 +9987,7 @@
       <c r="I12">
         <v>10</v>
       </c>
-      <c r="J12" s="2">
+      <c r="J12">
         <v>2024</v>
       </c>
       <c r="K12" t="s">
@@ -10027,7 +10022,7 @@
       <c r="I13">
         <v>10</v>
       </c>
-      <c r="J13" s="2">
+      <c r="J13">
         <v>2024</v>
       </c>
       <c r="K13" t="s">
@@ -10062,7 +10057,7 @@
       <c r="I14">
         <v>10</v>
       </c>
-      <c r="J14" s="2">
+      <c r="J14">
         <v>2024</v>
       </c>
       <c r="K14" t="s">
@@ -10097,7 +10092,7 @@
       <c r="I15">
         <v>10</v>
       </c>
-      <c r="J15" s="2">
+      <c r="J15">
         <v>2019</v>
       </c>
       <c r="K15" t="s">
@@ -10132,7 +10127,7 @@
       <c r="I16">
         <v>10</v>
       </c>
-      <c r="J16" s="2">
+      <c r="J16">
         <v>2025</v>
       </c>
       <c r="K16" t="s">
@@ -10167,7 +10162,7 @@
       <c r="I17">
         <v>10</v>
       </c>
-      <c r="J17" s="2">
+      <c r="J17">
         <v>2025</v>
       </c>
       <c r="K17" t="s">
@@ -10202,7 +10197,7 @@
       <c r="I18">
         <v>10</v>
       </c>
-      <c r="J18" s="2">
+      <c r="J18">
         <v>2018</v>
       </c>
       <c r="K18" t="s">
@@ -10237,7 +10232,7 @@
       <c r="I19">
         <v>10</v>
       </c>
-      <c r="J19" s="2">
+      <c r="J19">
         <v>2021</v>
       </c>
       <c r="K19" t="s">
@@ -10272,7 +10267,7 @@
       <c r="I20">
         <v>10</v>
       </c>
-      <c r="J20" s="2">
+      <c r="J20">
         <v>2021</v>
       </c>
       <c r="K20" t="s">
@@ -10307,7 +10302,7 @@
       <c r="I21">
         <v>10</v>
       </c>
-      <c r="J21" s="2">
+      <c r="J21">
         <v>2025</v>
       </c>
       <c r="K21" t="s">
@@ -10342,7 +10337,7 @@
       <c r="I22">
         <v>10</v>
       </c>
-      <c r="J22" s="2">
+      <c r="J22">
         <v>2025</v>
       </c>
       <c r="K22" t="s">
@@ -10377,7 +10372,7 @@
       <c r="I23">
         <v>10</v>
       </c>
-      <c r="J23" s="2">
+      <c r="J23">
         <v>2022</v>
       </c>
       <c r="K23" t="s">
@@ -10412,7 +10407,7 @@
       <c r="I24">
         <v>6</v>
       </c>
-      <c r="J24" s="2">
+      <c r="J24">
         <v>2022</v>
       </c>
       <c r="K24" t="s">
@@ -10447,7 +10442,7 @@
       <c r="I25">
         <v>6</v>
       </c>
-      <c r="J25" s="2">
+      <c r="J25">
         <v>2022</v>
       </c>
       <c r="K25" t="s">
@@ -10482,7 +10477,7 @@
       <c r="I26">
         <v>48</v>
       </c>
-      <c r="J26" s="2">
+      <c r="J26">
         <v>2015</v>
       </c>
       <c r="K26" t="s">
@@ -10517,7 +10512,7 @@
       <c r="I27">
         <v>48</v>
       </c>
-      <c r="J27" s="2">
+      <c r="J27">
         <v>2015</v>
       </c>
       <c r="K27" t="s">
@@ -10552,7 +10547,7 @@
       <c r="I28">
         <v>48</v>
       </c>
-      <c r="J28" s="2">
+      <c r="J28">
         <v>2015</v>
       </c>
       <c r="K28" t="s">
@@ -10587,7 +10582,7 @@
       <c r="I29">
         <v>48</v>
       </c>
-      <c r="J29" s="2">
+      <c r="J29">
         <v>2015</v>
       </c>
       <c r="K29" t="s">
@@ -10622,7 +10617,7 @@
       <c r="I30">
         <v>48</v>
       </c>
-      <c r="J30" s="2">
+      <c r="J30">
         <v>2015</v>
       </c>
       <c r="K30" t="s">
@@ -10657,7 +10652,7 @@
       <c r="I31">
         <v>48</v>
       </c>
-      <c r="J31" s="2">
+      <c r="J31">
         <v>2015</v>
       </c>
       <c r="K31" t="s">
@@ -10692,7 +10687,7 @@
       <c r="I32">
         <v>48</v>
       </c>
-      <c r="J32" s="2">
+      <c r="J32">
         <v>2015</v>
       </c>
       <c r="K32" t="s">
@@ -10727,7 +10722,7 @@
       <c r="I33">
         <v>48</v>
       </c>
-      <c r="J33" s="2">
+      <c r="J33">
         <v>2018</v>
       </c>
       <c r="K33" t="s">

</xml_diff>